<commit_message>
Added an excel column to object converter
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="test" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -58,6 +58,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -117,8 +118,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -254,30 +259,30 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>